<commit_message>
fix header is yes/no
</commit_message>
<xml_diff>
--- a/dataconfig/title.xlsx
+++ b/dataconfig/title.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="82">
   <si>
     <t>Title</t>
   </si>
@@ -33,238 +33,235 @@
     <t>img_content</t>
   </si>
   <si>
-    <t>Bibox庆生热烈进行中 200万大奖持续发放</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/news/bitcoin/276075.html</t>
-  </si>
-  <si>
-    <t>当然，打铁海的自身硬，Bibox今天的成就也少不了自身的努力。全球第一款人工智能交易所，流畅的交易体验、安全的资产管理、防作弊机制，一流的投资策略等等。</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1343225_image1.png</t>
-  </si>
-  <si>
-    <t>比特币暴跌能抄底吗？</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/member/175102</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1311318_image1.png</t>
-  </si>
-  <si>
-    <t>从进化论的思想说量化交易</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/bitcoin/276074.html</t>
-  </si>
-  <si>
-    <t>同时大家有想法或者有自己一套赚钱思路，不妨找一下客服，共享一下您的想法，可能币圈的韭菜因你的想法或者策略收益，走出人生地谷，迈向巅峰！！！</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1343236_image1.png</t>
-  </si>
-  <si>
-    <t>Angular 垮台、ES6 最受欢迎20,000 名程序员告诉你谁是 JS 王者</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/member/208299</t>
-  </si>
-  <si>
-    <t>任何能够用 JavaScript 实现的应用，最终都必将用 JavaScript 实现。</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1343200_image1.png</t>
-  </si>
-  <si>
-    <t>文化产业+区块链技术应用创新峰会 暨文产商城系统改版（文版通）上线说明会</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/bitcoin/276073.html</t>
-  </si>
-  <si>
-    <t>2018年11月20日，由深圳文化产权交易所、数字创意创新发展中心（文化艺术品版权区块链应用基地）、大数据国家工程实验室深圳文交所区块链应用中心共同举办的“文化</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1343207_image1.png</t>
-  </si>
-  <si>
-    <t>Mcoin推出资产管理平台 帮助MNT持有者收益最大化</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/member/204239</t>
-  </si>
-  <si>
-    <t>Mcoin交易所近期计划上线资产管理平台，帮助用户实现其数字资产的保值增值。具体上线时间，请见Mcoin交易所官方公告。（官方网址：www.mdex.mn)</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1343167_image1.png</t>
-  </si>
-  <si>
-    <t>区块链或成公关照妖镜？</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/bitcoin/276068.html</t>
-  </si>
-  <si>
-    <t>在区块链这面照妖镜下，那些虚假的妖魔鬼怪也只能原形毕露了。区块链在国内发展至今早已从单一的数字金融货币应用衍生至其他行业领域。在区块链的这片深海里，海面平静下，</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1343173_image1.png</t>
-  </si>
-  <si>
-    <t>BCH可能是个没有结局的故事</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/member/102673</t>
-  </si>
-  <si>
-    <t>大佬战斗，矿工操纵，韭菜接盘</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1343146_image1.png</t>
-  </si>
-  <si>
-    <t>BCH硬分叉闹剧未落幕  谁能是赢家</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/bitcoin/276070.html</t>
-  </si>
-  <si>
-    <t>好多小伙伴手痒忍不住想进场了，看来市场的恐慌情绪也逐渐恢复。不过没到我认为的很好的时机，所以我会暂时观望。</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1335046_image1.png</t>
-  </si>
-  <si>
-    <t>比特币价格跌破5000美元 科技股暴跌  背后原因是什么？</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/member/210243</t>
-  </si>
-  <si>
-    <t>区块链市场（Appasst）app，进入区块链的第一款APP。</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1343153_image1.png</t>
-  </si>
-  <si>
-    <t>关注1-2天内的走势  有机会走出底部形态</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/bitcoin/276069.html</t>
-  </si>
-  <si>
-    <t>保持密切关注接下来的1-2天，有机会形成一个底部形态。我们可以尝试进场，不过也是一样，毕竟大熊市，小玩即可。</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1340800_image1.png</t>
-  </si>
-  <si>
-    <t>五家对冲基金指控OKEx、在BCH分叉之际操纵合约规则</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/member/171533</t>
-  </si>
-  <si>
-    <t>处理与加密货币相关的衍生品为交易所开辟了新的商机。在OKEx的所有案例之中而言，该公司正面临着更多的审查。它最近修改了有关衍生品合约的条款，这突出表明需要对这些</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1343127_image1.png</t>
-  </si>
-  <si>
-    <t>（11.20行情分析）SEC对违规I西欧民事处罚   投资者被保护</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/bitcoin/276067.html</t>
-  </si>
-  <si>
-    <t>今日看什么---SEC对违规I西欧民事处罚</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1190720_image1.png</t>
-  </si>
-  <si>
-    <t>深度解析新一代的虚拟数字货币的典范：娱乐链YLS</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/member/209198</t>
-  </si>
-  <si>
-    <t>娱乐链YLS是基于以太坊ERC20智能合约协议产生，用户可以使用imtoken等轻钱包即可保管、存储与转发，是新一代的虚拟数字货币的典范。</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1343138_image1.png</t>
-  </si>
-  <si>
-    <t>LINFINITY CEO Anndy Lian：区块链赋能供应链重在落地</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/bitcoin/276066.html</t>
-  </si>
-  <si>
-    <t>供应链越长越复杂，欺诈和渎职的机会就越大。LINFINITY CEO Anndy Lian指出，传统供应链不安全，而区块链有潜力帮助供应链进行更透明更具穿透力的管理。</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1315750_image1.png</t>
-  </si>
-  <si>
-    <t>区块链夺宝游戏《ETH90》即将上线公测 参与公测赢取100个以太坊</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/member/163557</t>
-  </si>
-  <si>
-    <t>在这里希望《ETH90》上线公测大火！</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1343114_image1.png</t>
-  </si>
-  <si>
-    <t>EOS GO发布1周年</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/bitcoin/276065.html</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1343125_image1.png</t>
-  </si>
-  <si>
-    <t>BT110|比特币暴跌创新低 它是一场数字货币骗局吗？</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/member/155049</t>
-  </si>
-  <si>
-    <t>BT110：比特币暴跌创新低，它是一场数字货币骗局吗？</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1343123_image1.png</t>
-  </si>
-  <si>
-    <t>TBG Insights | 报复性反弹随时产生这将是中期内最有力量的多方声音</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/bitcoin/276064.html</t>
-  </si>
-  <si>
-    <t>面对币圈的瀑布，还是有人选择逆流而上，那么币圈接下来的走势会如他所料吗？</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1343101_image1.png</t>
-  </si>
-  <si>
-    <t>11. 20 行情分析：6000 5000 4500 加速下跌 共识砸盘？</t>
-  </si>
-  <si>
-    <t>https://www.jinse.com/member/191256</t>
-  </si>
-  <si>
-    <t>惨烈的一天</t>
-  </si>
-  <si>
-    <t>https://img.jinse.com/1343118_image1.png</t>
+    <t>是捍卫言论自由还是整顿网络暴力</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/bitcoin/276430.html</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1345469_image1.png</t>
+  </si>
+  <si>
+    <t>区块链十年 | 第1.2章  2008 比特币白皮书</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/member/208800</t>
+  </si>
+  <si>
+    <t>在世界的某个角落里，中本聪开发的第一版比特币客户端也即将完成。</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1345449_image1.png</t>
+  </si>
+  <si>
+    <t>懂个币 BSV扛不住了？算力战已让矿工损失数百万美元收入</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/bitcoin/276429.html</t>
+  </si>
+  <si>
+    <t>算力战让矿工损失数百万美元收入。</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1343898_image1.png</t>
+  </si>
+  <si>
+    <t>4分钟课堂 | 经济泡沫是如何产生的？</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/member/190014</t>
+  </si>
+  <si>
+    <t>自17世纪荷兰“郁金香狂热”事件成为第一场经济泡沫后，市场涌现出房地产泡沫 、股市泡沫、互联网泡沫、甚至比特币泡沫等各种经济泡沫。经济学家将经济泡沫分为五个阶段</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1345452_image1.png</t>
+  </si>
+  <si>
+    <t>区块链十年 | 第1.1章  2008 世界金融危机</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/bitcoin/276173.html</t>
+  </si>
+  <si>
+    <t>面对金融危机，一位神秘人思考着自己的解决方案......</t>
+  </si>
+  <si>
+    <t>2018.11.21 今日早盘短线策略 遵守规则敬畏市场</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/member/211555</t>
+  </si>
+  <si>
+    <t>2018.11.21 早间策略一览</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1298737_image1.png</t>
+  </si>
+  <si>
+    <t>哈希派：多头反弹软绵绵、但空头也想休息一下了</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/bitcoin/276427.html</t>
+  </si>
+  <si>
+    <t>今日行情分析币种：BTC / ETH / EOS / BCH / XRP / LTC</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1330734_image1.png</t>
+  </si>
+  <si>
+    <t>万点财经熊市专栏|陶太胜的熊市生存法则</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/member/202987</t>
+  </si>
+  <si>
+    <t>我本尘埃，因花而来</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1345385_image1.png</t>
+  </si>
+  <si>
+    <t>加密货币市值24小时蒸发2600亿“避险属性”丧失共识肢解？</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/bitcoin/276426.html</t>
+  </si>
+  <si>
+    <t>这场暴跌背后，有更深层的原因和更深远的影响。</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1343868_image1.png</t>
+  </si>
+  <si>
+    <t>走进区块链企业 | 赵伟：冬天很冷但我们很感谢这个冬天</t>
+  </si>
+  <si>
+    <t>这是一家走进去，便想细细去探索一番的企业</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1343833_image1.png</t>
+  </si>
+  <si>
+    <t>人工智能与区块链的边界逐渐模糊，软硬件将如何结合？</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/bitcoin/276425.html</t>
+  </si>
+  <si>
+    <t>2018年11月18日，2018比原链全球开发者大会在杭州国际博览中心（G20会馆）继续进行，这是杭州第一次由开源组织举办的技术型峰会，也是杭州被誉为区块链之城以来规模最大的一场区块链开发者</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1345437_image1.png</t>
+  </si>
+  <si>
+    <t>OGC第一款DAPP即将震撼来袭</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/member/208546</t>
+  </si>
+  <si>
+    <t>DAPP是OGC技术应用落地的第一步，也是其对全球网游行业颠覆之路的正式实施。</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1345335_image1.png</t>
+  </si>
+  <si>
+    <t>兄弟们秋裤不顶事了棉裤穿上吧</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/bitcoin/276424.html</t>
+  </si>
+  <si>
+    <t>矿机论斤卖。</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1343806_image1.png</t>
+  </si>
+  <si>
+    <t>AiBiChain创始人刘靖中入围“2018中国创新榜样人物”</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/member/26030</t>
+  </si>
+  <si>
+    <t>作为数字技术的前沿，近年来区块链技术在许多国家受到越来越多的关注。在中国，区块链与其他几个重要新技术一并被列为《“十三五”国家信息化规划》中的“重大任务和重点</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1345305_image1.png</t>
+  </si>
+  <si>
+    <t>网信办主管媒体针对区块链连发8文：肯定Token价值 落地应用是重点</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/bitcoin/276423.html</t>
+  </si>
+  <si>
+    <t>结合区块链目前“遇冷”的行业背景，或许可从这几篇组稿以一窥网信办等国家机构现阶段对于区块链的立场和态度。</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1345340_image1.png</t>
+  </si>
+  <si>
+    <t>“大崩盘”过后策略抄底的机会来了</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/member/142128</t>
+  </si>
+  <si>
+    <t>捡垃圾的时候到了</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1343795_image1.png</t>
+  </si>
+  <si>
+    <t>谁也没有想到 区块链还能用来熬鸡汤</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/bitcoin/276169.html</t>
+  </si>
+  <si>
+    <t>希望这是币圈人熬的最后一碗“鸡汤”。</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1345343_image1.png</t>
+  </si>
+  <si>
+    <t>币易Coinyee.io交易所1周年 百万Token大派送 100%有礼</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/member/126549</t>
+  </si>
+  <si>
+    <t>为感谢广大用户朋友们一直以来的陪伴与支持，币易Coinyee.io特借助1周年生日的机会，举办了一场价值百万元Token好礼派送活动，100%有礼！</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1345140_image1.png</t>
+  </si>
+  <si>
+    <t>英雄会聚 恰逢其时 元界CTO陈浩受邀参加Money20/20峰会圆桌会议 共话区块链最新趋势</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/bitcoin/276163.html</t>
+  </si>
+  <si>
+    <t>元界CTO陈浩受Money20/20主办方邀请参与圆桌会谈环节与全球“重量级”演讲嘉宾就如何打造金融区块链进行了深入的交流探讨。</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1345331_image1.png</t>
+  </si>
+  <si>
+    <t>NVIDIA Q3盈利报告印证了加密货币采矿业务正在枯竭</t>
+  </si>
+  <si>
+    <t>https://www.jinse.com/member/214042</t>
+  </si>
+  <si>
+    <t>美国芯片龙头科技公司NVIDIA在2018年11月15日发布了2018年第三季度财报。该报告指出</t>
+  </si>
+  <si>
+    <t>https://img.jinse.com/1343723_image1.png</t>
   </si>
 </sst>
 </file>
@@ -1275,21 +1272,21 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -1334,217 +1331,217 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>38</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>41</v>
-      </c>
-      <c r="C11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
         <v>44</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>45</v>
-      </c>
-      <c r="C12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
         <v>48</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>49</v>
-      </c>
-      <c r="C13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
         <v>52</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
         <v>53</v>
-      </c>
-      <c r="C14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
         <v>56</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>57</v>
-      </c>
-      <c r="C15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
         <v>60</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>61</v>
-      </c>
-      <c r="C16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
         <v>64</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>65</v>
-      </c>
-      <c r="C17" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
         <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
         <v>71</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>72</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>73</v>
-      </c>
-      <c r="D19" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
         <v>75</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>76</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>77</v>
-      </c>
-      <c r="D20" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" t="s">
         <v>79</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>80</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>81</v>
-      </c>
-      <c r="D21" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>